<commit_message>
islem bedeli sutunu eklendi
</commit_message>
<xml_diff>
--- a/etikom/static/file/ornek-kargo-dosyasi.xlsx
+++ b/etikom/static/file/ornek-kargo-dosyasi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oktay\Desktop\emuhasebe\etikom\static\file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oktay\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198C866C-27E0-4862-BBF5-F8E463D8956A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC51FD8-029D-4B39-9503-166E7124799E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{86F3079F-4753-4881-B42E-C7974ACE6E2B}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Sipariş No</t>
   </si>
@@ -198,7 +198,10 @@
     <t>Kargo Tutarı</t>
   </si>
   <si>
-    <t>Hizmet + İşlem Bedeli</t>
+    <t>Hizmet Bedeli</t>
+  </si>
+  <si>
+    <t>İşlem Bedeli</t>
   </si>
 </sst>
 </file>
@@ -594,7 +597,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F2A9167-9377-494C-AB4F-1FE7F20C4B14}">
-  <dimension ref="A1:D204"/>
+  <dimension ref="A1:E204"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
@@ -603,11 +606,11 @@
     <col min="1" max="1" width="23.89453125" style="2" customWidth="1"/>
     <col min="2" max="2" width="13.20703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.7890625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.89453125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.15625" style="1"/>
+    <col min="4" max="5" width="19.89453125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.15625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -620,8 +623,11 @@
       <c r="D1" s="6" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E1" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2">
         <v>103378891</v>
       </c>
@@ -634,8 +640,11 @@
       <c r="D2" s="7">
         <v>3.89</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E2" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2">
         <v>253084405</v>
       </c>
@@ -648,8 +657,11 @@
       <c r="D3" s="7">
         <v>3.89</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E3" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>46</v>
       </c>
@@ -662,8 +674,11 @@
       <c r="D4" s="7">
         <v>2.4500000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E4" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>47</v>
       </c>
@@ -676,8 +691,11 @@
       <c r="D5" s="7">
         <v>2.4500000000000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E5" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
         <v>48</v>
       </c>
@@ -690,8 +708,11 @@
       <c r="D6" s="7">
         <v>2.4500000000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E6" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
         <v>49</v>
       </c>
@@ -704,8 +725,11 @@
       <c r="D7" s="7">
         <v>2.4500000000000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E7" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
         <v>53</v>
       </c>
@@ -718,8 +742,11 @@
       <c r="D8" s="7">
         <v>4.99</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E8" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
         <v>50</v>
       </c>
@@ -732,8 +759,11 @@
       <c r="D9" s="7">
         <v>4.99</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E9" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
         <v>52</v>
       </c>
@@ -746,8 +776,11 @@
       <c r="D10" s="7">
         <v>4.99</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E10" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
@@ -760,8 +793,11 @@
       <c r="D11" s="7">
         <v>4.99</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E11" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2">
         <v>1026904729</v>
       </c>
@@ -774,8 +810,11 @@
       <c r="D12" s="7">
         <v>13.4</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E12" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2">
         <v>3014287220</v>
       </c>
@@ -788,8 +827,11 @@
       <c r="D13" s="7">
         <v>13.4</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E13" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2">
         <v>4133852021</v>
       </c>
@@ -802,8 +844,11 @@
       <c r="D14" s="7">
         <v>13.4</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E14" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2">
         <v>6820774839</v>
       </c>
@@ -816,8 +861,11 @@
       <c r="D15" s="7">
         <v>13.4</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E15" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2">
         <v>1133852021</v>
       </c>
@@ -830,8 +878,11 @@
       <c r="D16" s="7">
         <v>13.4</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E16" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2">
         <v>517710605</v>
       </c>
@@ -844,8 +895,11 @@
       <c r="D17" s="7">
         <v>6.78</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E17" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2">
         <v>333452346</v>
       </c>
@@ -858,8 +912,11 @@
       <c r="D18" s="7">
         <v>6.78</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E18" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2">
         <v>678342346</v>
       </c>
@@ -872,8 +929,11 @@
       <c r="D19" s="7">
         <v>6.78</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E19" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2">
         <v>123578045</v>
       </c>
@@ -886,8 +946,11 @@
       <c r="D20" s="7">
         <v>6.78</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E20" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2">
         <v>956423677</v>
       </c>
@@ -900,8 +963,11 @@
       <c r="D21" s="7">
         <v>6.78</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E21" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2">
         <v>134214508</v>
       </c>
@@ -914,8 +980,11 @@
       <c r="D22" s="7">
         <v>3.79</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E22" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2">
         <v>736742133</v>
       </c>
@@ -928,8 +997,11 @@
       <c r="D23" s="7">
         <v>3.79</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E23" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
@@ -942,8 +1014,11 @@
       <c r="D24" s="7">
         <v>3.79</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E24" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2" t="s">
         <v>25</v>
       </c>
@@ -956,8 +1031,11 @@
       <c r="D25" s="7">
         <v>3.79</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E25" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
@@ -970,8 +1048,11 @@
       <c r="D26" s="7">
         <v>3.79</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E26" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2" t="s">
         <v>27</v>
       </c>
@@ -984,8 +1065,11 @@
       <c r="D27" s="7">
         <v>3.79</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E27" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
@@ -998,8 +1082,11 @@
       <c r="D28" s="7">
         <v>3.79</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E28" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2" t="s">
         <v>29</v>
       </c>
@@ -1012,8 +1099,11 @@
       <c r="D29" s="7">
         <v>3.79</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E29" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2" t="s">
         <v>30</v>
       </c>
@@ -1026,8 +1116,11 @@
       <c r="D30" s="7">
         <v>3.79</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E30" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
@@ -1040,8 +1133,11 @@
       <c r="D31" s="7">
         <v>3.79</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E31" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2" t="s">
         <v>32</v>
       </c>
@@ -1054,8 +1150,11 @@
       <c r="D32" s="7">
         <v>3.79</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E32" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2" t="s">
         <v>33</v>
       </c>
@@ -1068,8 +1167,11 @@
       <c r="D33" s="7">
         <v>3.79</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E33" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
@@ -1082,8 +1184,11 @@
       <c r="D34" s="7">
         <v>4.99</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E34" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2" t="s">
         <v>35</v>
       </c>
@@ -1096,8 +1201,11 @@
       <c r="D35" s="7">
         <v>4.99</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E35" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2" t="s">
         <v>36</v>
       </c>
@@ -1110,8 +1218,11 @@
       <c r="D36" s="7">
         <v>4.99</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E36" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2" t="s">
         <v>37</v>
       </c>
@@ -1124,8 +1235,11 @@
       <c r="D37" s="7">
         <v>4.99</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E37" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="2" t="s">
         <v>38</v>
       </c>
@@ -1138,8 +1252,11 @@
       <c r="D38" s="7">
         <v>4.99</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E38" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="2" t="s">
         <v>39</v>
       </c>
@@ -1152,8 +1269,11 @@
       <c r="D39" s="7">
         <v>4.99</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E39" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="2" t="s">
         <v>40</v>
       </c>
@@ -1166,8 +1286,11 @@
       <c r="D40" s="7">
         <v>4.99</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E40" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="2" t="s">
         <v>41</v>
       </c>
@@ -1180,8 +1303,11 @@
       <c r="D41" s="7">
         <v>4.99</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E41" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="2" t="s">
         <v>1</v>
       </c>
@@ -1194,8 +1320,11 @@
       <c r="D42" s="7">
         <v>12.55</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E42" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="2" t="s">
         <v>2</v>
       </c>
@@ -1208,8 +1337,11 @@
       <c r="D43" s="7">
         <v>12.55</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E43" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="2" t="s">
         <v>3</v>
       </c>
@@ -1222,8 +1354,11 @@
       <c r="D44" s="7">
         <v>12.55</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E44" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="2" t="s">
         <v>4</v>
       </c>
@@ -1236,8 +1371,11 @@
       <c r="D45" s="7">
         <v>12.55</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E45" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="2" t="s">
         <v>5</v>
       </c>
@@ -1250,8 +1388,11 @@
       <c r="D46" s="7">
         <v>12.55</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E46" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="2" t="s">
         <v>6</v>
       </c>
@@ -1264,8 +1405,11 @@
       <c r="D47" s="7">
         <v>12.55</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E47" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="2" t="s">
         <v>7</v>
       </c>
@@ -1278,8 +1422,11 @@
       <c r="D48" s="7">
         <v>12.55</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E48" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="2" t="s">
         <v>8</v>
       </c>
@@ -1292,8 +1439,11 @@
       <c r="D49" s="7">
         <v>12.55</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E49" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="2" t="s">
         <v>9</v>
       </c>
@@ -1306,8 +1456,11 @@
       <c r="D50" s="7">
         <v>12.55</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E50" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="2" t="s">
         <v>10</v>
       </c>
@@ -1320,8 +1473,11 @@
       <c r="D51" s="7">
         <v>9.9</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E51" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="2" t="s">
         <v>11</v>
       </c>
@@ -1334,8 +1490,11 @@
       <c r="D52" s="7">
         <v>9.9</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E52" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="2" t="s">
         <v>12</v>
       </c>
@@ -1348,8 +1507,11 @@
       <c r="D53" s="7">
         <v>9.9</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E53" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="2" t="s">
         <v>13</v>
       </c>
@@ -1362,8 +1524,11 @@
       <c r="D54" s="7">
         <v>9.9</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E54" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="2" t="s">
         <v>14</v>
       </c>
@@ -1376,8 +1541,11 @@
       <c r="D55" s="7">
         <v>9.9</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E55" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="2" t="s">
         <v>15</v>
       </c>
@@ -1390,8 +1558,11 @@
       <c r="D56" s="7">
         <v>9.9</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E56" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="2" t="s">
         <v>16</v>
       </c>
@@ -1404,8 +1575,11 @@
       <c r="D57" s="7">
         <v>9.9</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E57" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="2" t="s">
         <v>17</v>
       </c>
@@ -1418,8 +1592,11 @@
       <c r="D58" s="7">
         <v>9.9</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E58" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -1432,8 +1609,11 @@
       <c r="D59" s="7">
         <v>9.9</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E59" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="2">
         <v>2220804779</v>
       </c>
@@ -1446,8 +1626,11 @@
       <c r="D60" s="7">
         <v>11.1</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E60" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="2" t="s">
         <v>19</v>
       </c>
@@ -1460,8 +1643,11 @@
       <c r="D61" s="7">
         <v>11.1</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E61" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="2" t="s">
         <v>20</v>
       </c>
@@ -1474,8 +1660,11 @@
       <c r="D62" s="7">
         <v>11.1</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E62" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="2" t="s">
         <v>21</v>
       </c>
@@ -1488,8 +1677,11 @@
       <c r="D63" s="7">
         <v>11.1</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E63" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="2" t="s">
         <v>22</v>
       </c>
@@ -1502,8 +1694,11 @@
       <c r="D64" s="7">
         <v>11.1</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E64" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="2" t="s">
         <v>23</v>
       </c>
@@ -1516,8 +1711,11 @@
       <c r="D65" s="7">
         <v>11.1</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E65" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="2">
         <v>43108801</v>
       </c>
@@ -1530,8 +1728,11 @@
       <c r="D66" s="7">
         <v>11.1</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E66" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="2">
         <v>85234553</v>
       </c>
@@ -1544,8 +1745,11 @@
       <c r="D67" s="7">
         <v>11.1</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E67" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="2">
         <v>22623665</v>
       </c>
@@ -1558,8 +1762,11 @@
       <c r="D68" s="7">
         <v>11.1</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E68" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="2">
         <v>71102057</v>
       </c>
@@ -1572,8 +1779,11 @@
       <c r="D69" s="7">
         <v>7.43</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E69" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="2" t="s">
         <v>42</v>
       </c>
@@ -1586,8 +1796,11 @@
       <c r="D70" s="7">
         <v>7.43</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E70" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="2" t="s">
         <v>43</v>
       </c>
@@ -1600,8 +1813,11 @@
       <c r="D71" s="7">
         <v>7.43</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E71" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="2" t="s">
         <v>44</v>
       </c>
@@ -1614,8 +1830,11 @@
       <c r="D72" s="7">
         <v>7.43</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E72" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="2" t="s">
         <v>45</v>
       </c>
@@ -1628,8 +1847,11 @@
       <c r="D73" s="7">
         <v>7.43</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E73" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="2">
         <v>3506164310</v>
       </c>
@@ -1642,8 +1864,11 @@
       <c r="D74" s="7">
         <v>9.4499999999999993</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E74" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="2">
         <v>8231004393</v>
       </c>
@@ -1656,121 +1881,142 @@
       <c r="D75" s="7">
         <v>9.4499999999999993</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E75" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B76" s="3"/>
       <c r="C76" s="5"/>
       <c r="D76" s="7"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E76" s="7"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A77"/>
       <c r="B77" s="3"/>
       <c r="C77" s="5"/>
       <c r="D77" s="7"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E77" s="7"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A78"/>
       <c r="B78" s="3"/>
       <c r="C78" s="5"/>
       <c r="D78" s="7"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E78" s="7"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A79"/>
       <c r="B79" s="3"/>
       <c r="C79" s="5"/>
       <c r="D79" s="7"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E79" s="7"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A80"/>
       <c r="B80" s="3"/>
       <c r="C80" s="5"/>
       <c r="D80" s="7"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E80" s="7"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A81"/>
       <c r="B81" s="3"/>
       <c r="C81" s="5"/>
       <c r="D81" s="7"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E81" s="7"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A82"/>
       <c r="B82" s="3"/>
       <c r="C82" s="4"/>
       <c r="D82" s="7"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E82" s="7"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A83"/>
       <c r="B83" s="3"/>
       <c r="C83" s="5"/>
       <c r="D83" s="7"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E83" s="7"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A84"/>
       <c r="B84" s="3"/>
       <c r="C84" s="5"/>
       <c r="D84" s="7"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E84" s="7"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A85"/>
       <c r="B85" s="3"/>
       <c r="C85" s="5"/>
       <c r="D85" s="7"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E85" s="7"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A86"/>
       <c r="B86" s="3"/>
       <c r="C86" s="5"/>
       <c r="D86" s="7"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E86" s="7"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A87"/>
       <c r="B87" s="3"/>
       <c r="C87" s="5"/>
       <c r="D87" s="7"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E87" s="7"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A88"/>
       <c r="B88" s="3"/>
       <c r="C88" s="5"/>
       <c r="D88" s="7"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E88" s="7"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A89"/>
       <c r="B89" s="3"/>
       <c r="C89" s="5"/>
       <c r="D89" s="7"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E89" s="7"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A90"/>
       <c r="B90" s="3"/>
       <c r="C90" s="5"/>
       <c r="D90" s="7"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E90" s="7"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A91"/>
       <c r="B91" s="3"/>
       <c r="C91" s="5"/>
       <c r="D91" s="7"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E91" s="7"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A92"/>
       <c r="B92" s="3"/>
       <c r="C92" s="5"/>
       <c r="D92" s="7"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E92" s="7"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A93"/>
       <c r="B93" s="3"/>
       <c r="C93" s="5"/>
       <c r="D93" s="7"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E93" s="7"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A94"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A95"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A96"/>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -2101,5 +2347,8 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="A24 A25:A42 A43:A65 A70:A73" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>